<commit_message>
add index startend headers cells ...
</commit_message>
<xml_diff>
--- a/example_excel.xlsx
+++ b/example_excel.xlsx
@@ -200,7 +200,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -402,6 +402,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -410,43 +422,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -730,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,70 +881,70 @@
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -985,45 +966,45 @@
       <c r="P7" s="15"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21" t="s">
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="16" t="s">
         <v>34</v>
       </c>
@@ -1063,10 +1044,10 @@
       <c r="B10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="19">
         <v>4156.4560000000001</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>123456789.123</v>
       </c>
       <c r="E10" s="11"/>
@@ -1075,7 +1056,7 @@
       <c r="H10" s="11">
         <v>4564</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="21">
         <v>-12345678912.1</v>
       </c>
       <c r="J10" s="11"/>
@@ -1097,7 +1078,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="24"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="11"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -1119,7 +1100,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="24"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="11"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -1139,7 +1120,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="24"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="11"/>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -1161,7 +1142,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="24"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="11"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -1181,7 +1162,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="24"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="11"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
@@ -1201,7 +1182,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="24"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="11"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -1221,7 +1202,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
-      <c r="I17" s="24"/>
+      <c r="I17" s="21"/>
       <c r="J17" s="11"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -1241,7 +1222,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
-      <c r="I18" s="24"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="11"/>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -1261,7 +1242,7 @@
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="11"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -1281,7 +1262,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
-      <c r="I20" s="24"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="11"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -1301,7 +1282,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="24"/>
+      <c r="I21" s="21"/>
       <c r="J21" s="11"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
@@ -1321,7 +1302,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="24"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="11"/>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -1341,7 +1322,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="24"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="11"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
@@ -1361,7 +1342,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="24"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="11"/>
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
@@ -1383,7 +1364,7 @@
     <mergeCell ref="B5:P5"/>
   </mergeCells>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$C$2=c_amounts</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
we are with formats
</commit_message>
<xml_diff>
--- a/example_excel.xlsx
+++ b/example_excel.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="only_table" sheetId="1" r:id="rId1"/>
+    <sheet name="info" sheetId="2" r:id="rId2"/>
+    <sheet name="table_with_info" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>C1</t>
   </si>
@@ -348,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,12 +423,20 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -709,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,338 +736,230 @@
     <col min="16" max="16" width="2.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>50</v>
-      </c>
-      <c r="B3" s="2">
-        <v>200</v>
-      </c>
-      <c r="C3" s="2">
-        <v>100</v>
-      </c>
-      <c r="D3" s="2">
-        <v>120</v>
-      </c>
-      <c r="E3" s="2">
-        <v>120</v>
-      </c>
-      <c r="F3" s="2">
-        <v>120</v>
-      </c>
-      <c r="G3" s="2">
-        <v>120</v>
-      </c>
-      <c r="H3" s="2">
-        <v>120</v>
-      </c>
-      <c r="I3" s="2">
-        <v>120</v>
-      </c>
-      <c r="J3" s="2">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2">
-        <v>120</v>
-      </c>
-      <c r="L3" s="2">
-        <v>120</v>
-      </c>
-      <c r="M3" s="2">
-        <v>120</v>
-      </c>
-      <c r="N3" s="2">
-        <v>120</v>
-      </c>
-      <c r="O3" s="2">
-        <v>100</v>
-      </c>
-      <c r="P3" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="23" t="s">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="23" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C5" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25" t="s">
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="16" t="s">
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="N6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C7" s="19">
         <v>4156.4560000000001</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D7" s="20">
         <v>123456789.123</v>
       </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11">
+        <v>4564</v>
+      </c>
+      <c r="I7" s="21">
+        <v>-12345678912.1</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="11">
-        <v>4564</v>
-      </c>
-      <c r="I10" s="21">
-        <v>-12345678912.1</v>
-      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="11"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1068,11 +969,11 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>8</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10">
+        <v>4564</v>
+      </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -1087,13 +988,9 @@
       <c r="O11" s="10"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:16" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>9</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>44</v>
-      </c>
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -1110,9 +1007,7 @@
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>10</v>
-      </c>
+      <c r="A13" s="5"/>
       <c r="B13" s="12"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
@@ -1130,13 +1025,9 @@
       <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>11</v>
-      </c>
+      <c r="A14" s="5"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="10">
-        <v>4564</v>
-      </c>
+      <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1152,9 +1043,7 @@
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>12</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" s="12"/>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
@@ -1172,9 +1061,7 @@
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>13</v>
-      </c>
+      <c r="A16" s="5"/>
       <c r="B16" s="12"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -1192,9 +1079,7 @@
       <c r="P16" s="5"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>14</v>
-      </c>
+      <c r="A17" s="5"/>
       <c r="B17" s="12"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
@@ -1212,9 +1097,7 @@
       <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>15</v>
-      </c>
+      <c r="A18" s="5"/>
       <c r="B18" s="12"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
@@ -1232,9 +1115,7 @@
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>16</v>
-      </c>
+      <c r="A19" s="5"/>
       <c r="B19" s="12"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
@@ -1252,9 +1133,7 @@
       <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>17</v>
-      </c>
+      <c r="A20" s="5"/>
       <c r="B20" s="12"/>
       <c r="C20" s="10"/>
       <c r="D20" s="11"/>
@@ -1272,11 +1151,9 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>18</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -1284,88 +1161,28 @@
       <c r="H21" s="11"/>
       <c r="I21" s="21"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
       <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>19</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>20</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="B4:P4"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="K5:O5"/>
+    <mergeCell ref="B2:P2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$C$2=c_amounts</formula>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>#REF!=c_amounts</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1515,4 +1332,709 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="9" width="17.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="1" customWidth="1"/>
+    <col min="11" max="14" width="17.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2">
+        <v>200</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>120</v>
+      </c>
+      <c r="E3" s="2">
+        <v>120</v>
+      </c>
+      <c r="F3" s="2">
+        <v>120</v>
+      </c>
+      <c r="G3" s="2">
+        <v>120</v>
+      </c>
+      <c r="H3" s="2">
+        <v>120</v>
+      </c>
+      <c r="I3" s="2">
+        <v>120</v>
+      </c>
+      <c r="J3" s="2">
+        <v>100</v>
+      </c>
+      <c r="K3" s="2">
+        <v>120</v>
+      </c>
+      <c r="L3" s="2">
+        <v>120</v>
+      </c>
+      <c r="M3" s="2">
+        <v>120</v>
+      </c>
+      <c r="N3" s="2">
+        <v>120</v>
+      </c>
+      <c r="O3" s="2">
+        <v>100</v>
+      </c>
+      <c r="P3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="19">
+        <v>4156.4560000000001</v>
+      </c>
+      <c r="D10" s="20">
+        <v>123456789.123</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11">
+        <v>4564</v>
+      </c>
+      <c r="I10" s="21">
+        <v>-12345678912.1</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>8</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>9</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>11</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10">
+        <v>4564</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>13</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>14</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>17</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>18</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>19</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>20</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>21</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>22</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="K8:O8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C$2=c_amounts</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add normalcellloop and css format
</commit_message>
<xml_diff>
--- a/example_excel.xlsx
+++ b/example_excel.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.amrouche\Desktop\reacttableurproject\excel_to_handsontable\"/>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,6 +416,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -424,8 +427,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,10 +721,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,67 +742,67 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="15"/>
@@ -818,40 +822,40 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="16" t="s">
         <v>34</v>
       </c>
@@ -916,7 +920,7 @@
       <c r="A8" s="5"/>
       <c r="B8" s="17"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -937,7 +941,7 @@
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -1192,10 +1196,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil2"/>
   <dimension ref="C1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,6 +1341,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1508,67 +1514,67 @@
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
@@ -1596,42 +1602,42 @@
       <c r="A8" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25" t="s">
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="16" t="s">
         <v>34</v>
       </c>

</xml_diff>